<commit_message>
add excel measurements of snoring
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JELENA\FAKS\3.godina\6.semestar\zavrsni\zavrsni-rad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A98676-C670-4D90-9FF7-132089BC189C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1F3AD1-BB7D-486B-B3FB-39243635C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59AAA055-06BE-4089-858D-5DFDDCE26241}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>d/cm</t>
   </si>
@@ -53,13 +53,127 @@
   </si>
   <si>
     <t>f/Hz</t>
+  </si>
+  <si>
+    <t>FILE</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>č</t>
+  </si>
+  <si>
+    <t>ć</t>
+  </si>
+  <si>
+    <t>đ</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>ž</t>
+  </si>
+  <si>
+    <t>š</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>puno</t>
+  </si>
+  <si>
+    <t>svega</t>
+  </si>
+  <si>
+    <t>svasta</t>
+  </si>
+  <si>
+    <t>nesto</t>
+  </si>
+  <si>
+    <t>738~</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,8 +189,23 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +221,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -138,6 +285,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1584,10 +1750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AA949A-4943-4AB9-B017-E41F54B3B033}">
-  <dimension ref="F1:J22"/>
+  <dimension ref="F1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1799,7 +1965,7 @@
         <v>-41</v>
       </c>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F17">
         <v>15</v>
       </c>
@@ -1810,7 +1976,7 @@
         <v>-31</v>
       </c>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F18">
         <v>16</v>
       </c>
@@ -1821,7 +1987,7 @@
         <v>-47</v>
       </c>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F19">
         <v>17</v>
       </c>
@@ -1832,7 +1998,7 @@
         <v>-42</v>
       </c>
     </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F20">
         <v>18</v>
       </c>
@@ -1843,7 +2009,7 @@
         <v>-36</v>
       </c>
     </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F21">
         <v>19</v>
       </c>
@@ -1854,7 +2020,7 @@
         <v>-34</v>
       </c>
     </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F22">
         <v>20</v>
       </c>
@@ -1863,6 +2029,462 @@
       </c>
       <c r="H22" s="5">
         <v>-40</v>
+      </c>
+    </row>
+    <row r="24" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="L25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M25" s="7">
+        <v>1</v>
+      </c>
+      <c r="N25" s="7">
+        <v>2</v>
+      </c>
+      <c r="O25" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="L26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="1">
+        <v>230</v>
+      </c>
+      <c r="N26" s="9">
+        <v>474</v>
+      </c>
+      <c r="O26">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="27" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="L27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27" s="1">
+        <v>48</v>
+      </c>
+      <c r="N27" s="9">
+        <v>906</v>
+      </c>
+      <c r="O27">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="28" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="L28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" s="8">
+        <v>49</v>
+      </c>
+      <c r="N28" t="s">
+        <v>38</v>
+      </c>
+      <c r="O28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="L29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M29" s="8">
+        <v>590</v>
+      </c>
+      <c r="N29" t="s">
+        <v>38</v>
+      </c>
+      <c r="O29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="L30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="1">
+        <v>49</v>
+      </c>
+      <c r="N30">
+        <v>148</v>
+      </c>
+      <c r="O30" s="9">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="31" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="L31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M31" s="1">
+        <v>48</v>
+      </c>
+      <c r="N31">
+        <v>150</v>
+      </c>
+      <c r="O31" s="9">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="32" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="L32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M32" s="8">
+        <v>92</v>
+      </c>
+      <c r="N32" t="s">
+        <v>38</v>
+      </c>
+      <c r="O32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="1">
+        <v>48</v>
+      </c>
+      <c r="N33">
+        <v>145</v>
+      </c>
+      <c r="O33" s="9">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="34" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M34" s="1">
+        <v>45</v>
+      </c>
+      <c r="N34" s="1">
+        <v>676</v>
+      </c>
+      <c r="O34">
+        <v>1236</v>
+      </c>
+      <c r="P34" s="9">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="35" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M35" s="8">
+        <v>49</v>
+      </c>
+      <c r="N35">
+        <v>492</v>
+      </c>
+      <c r="O35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M36" s="1">
+        <v>44</v>
+      </c>
+      <c r="N36">
+        <v>145</v>
+      </c>
+      <c r="O36" s="9">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="37" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M37" s="1">
+        <v>45</v>
+      </c>
+      <c r="N37">
+        <v>144</v>
+      </c>
+      <c r="O37" s="9">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="38" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="1">
+        <v>48</v>
+      </c>
+      <c r="N38" s="9">
+        <v>502</v>
+      </c>
+      <c r="O38">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="39" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" s="1">
+        <v>49</v>
+      </c>
+      <c r="N39">
+        <v>505</v>
+      </c>
+      <c r="O39" s="9">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="40" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" s="8">
+        <v>602</v>
+      </c>
+      <c r="N40" t="s">
+        <v>38</v>
+      </c>
+      <c r="O40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M41" s="8">
+        <v>49</v>
+      </c>
+      <c r="N41">
+        <v>359</v>
+      </c>
+      <c r="O41">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="42" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42" s="8">
+        <v>49</v>
+      </c>
+      <c r="N42">
+        <v>475</v>
+      </c>
+      <c r="O42">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="43" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" s="1">
+        <v>48</v>
+      </c>
+      <c r="N43" s="9">
+        <v>501</v>
+      </c>
+      <c r="O43">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="44" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="8">
+        <v>49</v>
+      </c>
+      <c r="N44">
+        <v>88</v>
+      </c>
+      <c r="O44">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="45" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M45" s="1">
+        <v>48</v>
+      </c>
+      <c r="N45" s="9">
+        <v>501</v>
+      </c>
+      <c r="O45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L46" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N46" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+    </row>
+    <row r="47" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L47" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M47" s="10">
+        <v>78</v>
+      </c>
+      <c r="N47" s="12">
+        <v>145</v>
+      </c>
+      <c r="O47" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="P47" s="11"/>
+    </row>
+    <row r="48" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M48" s="1">
+        <v>48</v>
+      </c>
+      <c r="N48">
+        <v>592</v>
+      </c>
+      <c r="O48" s="9">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="49" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L49" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M49" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N49" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+    </row>
+    <row r="50" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L50" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M50" s="14">
+        <v>238</v>
+      </c>
+      <c r="N50" s="13">
+        <v>678</v>
+      </c>
+      <c r="O50" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="P50" s="13"/>
+    </row>
+    <row r="51" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M51" s="1">
+        <v>44</v>
+      </c>
+      <c r="N51">
+        <v>678</v>
+      </c>
+      <c r="O51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M52" s="1">
+        <v>48</v>
+      </c>
+      <c r="N52" s="9">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="53" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M53" s="1">
+        <v>48</v>
+      </c>
+      <c r="N53">
+        <v>145</v>
+      </c>
+      <c r="O53">
+        <v>456</v>
+      </c>
+      <c r="P53" s="9">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="54" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M54" s="1">
+        <v>48</v>
+      </c>
+      <c r="N54" t="s">
+        <v>38</v>
+      </c>
+      <c r="O54" s="9">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="55" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M55" s="8">
+        <v>49</v>
+      </c>
+      <c r="N55" t="s">
+        <v>38</v>
+      </c>
+      <c r="O55">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="56" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L56" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M56" s="1">
+        <v>84</v>
+      </c>
+      <c r="N56">
+        <v>500</v>
+      </c>
+      <c r="O56">
+        <v>908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change file structure, excel update
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JELENA\FAKS\3.godina\6.semestar\zavrsni\zavrsni-rad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1F3AD1-BB7D-486B-B3FB-39243635C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77B03FE-CBCC-475C-AE2F-098ABEFB29C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59AAA055-06BE-4089-858D-5DFDDCE26241}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>d/cm</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>738~</t>
+  </si>
+  <si>
+    <t>super!</t>
+  </si>
+  <si>
+    <t>NE VALJA</t>
   </si>
 </sst>
 </file>
@@ -205,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +248,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -270,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,11 +313,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1750,10 +1769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AA949A-4943-4AB9-B017-E41F54B3B033}">
-  <dimension ref="F1:P56"/>
+  <dimension ref="F1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1965,7 +1984,7 @@
         <v>-41</v>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F17">
         <v>15</v>
       </c>
@@ -1976,7 +1995,7 @@
         <v>-31</v>
       </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F18">
         <v>16</v>
       </c>
@@ -1987,7 +2006,7 @@
         <v>-47</v>
       </c>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F19">
         <v>17</v>
       </c>
@@ -1998,7 +2017,7 @@
         <v>-42</v>
       </c>
     </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F20">
         <v>18</v>
       </c>
@@ -2009,7 +2028,7 @@
         <v>-36</v>
       </c>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F21">
         <v>19</v>
       </c>
@@ -2020,7 +2039,7 @@
         <v>-34</v>
       </c>
     </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F22">
         <v>20</v>
       </c>
@@ -2031,12 +2050,12 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="24" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:16" x14ac:dyDescent="0.3">
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:16" x14ac:dyDescent="0.3">
       <c r="L25" s="6" t="s">
         <v>6</v>
       </c>
@@ -2050,7 +2069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:16" x14ac:dyDescent="0.3">
       <c r="L26" s="1" t="s">
         <v>7</v>
       </c>
@@ -2064,7 +2083,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:16" x14ac:dyDescent="0.3">
       <c r="L27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2078,7 +2097,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:16" x14ac:dyDescent="0.3">
       <c r="L28" s="1" t="s">
         <v>9</v>
       </c>
@@ -2092,7 +2111,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:16" x14ac:dyDescent="0.3">
       <c r="L29" s="1" t="s">
         <v>10</v>
       </c>
@@ -2105,8 +2124,11 @@
       <c r="O29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="P29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="6:16" x14ac:dyDescent="0.3">
       <c r="L30" s="1" t="s">
         <v>11</v>
       </c>
@@ -2120,7 +2142,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:16" x14ac:dyDescent="0.3">
       <c r="L31" s="1" t="s">
         <v>13</v>
       </c>
@@ -2134,7 +2156,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:16" x14ac:dyDescent="0.3">
       <c r="L32" s="1" t="s">
         <v>12</v>
       </c>
@@ -2148,7 +2170,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L33" s="1" t="s">
         <v>14</v>
       </c>
@@ -2162,7 +2184,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="34" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L34" s="1" t="s">
         <v>15</v>
       </c>
@@ -2179,7 +2201,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="35" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L35" s="1" t="s">
         <v>16</v>
       </c>
@@ -2193,7 +2215,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L36" s="1" t="s">
         <v>17</v>
       </c>
@@ -2207,7 +2229,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="37" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L37" s="1" t="s">
         <v>18</v>
       </c>
@@ -2221,7 +2243,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="38" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L38" s="1" t="s">
         <v>19</v>
       </c>
@@ -2235,7 +2257,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="39" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L39" s="1" t="s">
         <v>20</v>
       </c>
@@ -2249,7 +2271,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="40" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L40" s="1" t="s">
         <v>21</v>
       </c>
@@ -2262,8 +2284,11 @@
       <c r="O40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="P40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2277,7 +2302,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="42" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L42" s="1" t="s">
         <v>23</v>
       </c>
@@ -2291,7 +2316,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="43" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L43" s="1" t="s">
         <v>24</v>
       </c>
@@ -2305,7 +2330,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="44" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L44" s="1" t="s">
         <v>25</v>
       </c>
@@ -2319,7 +2344,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="45" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L45" s="1" t="s">
         <v>26</v>
       </c>
@@ -2333,7 +2358,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L46" s="10" t="s">
         <v>27</v>
       </c>
@@ -2346,22 +2371,25 @@
       <c r="O46" s="11"/>
       <c r="P46" s="11"/>
     </row>
-    <row r="47" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L47" s="10" t="s">
+    <row r="47" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L47" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="M47" s="10">
+      <c r="M47" s="15">
         <v>78</v>
       </c>
-      <c r="N47" s="12">
+      <c r="N47" s="16">
         <v>145</v>
       </c>
-      <c r="O47" s="11" t="s">
+      <c r="O47" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="P47" s="11"/>
-    </row>
-    <row r="48" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="P47" s="17"/>
+      <c r="Q47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L48" s="1" t="s">
         <v>37</v>
       </c>
@@ -2389,19 +2417,19 @@
       <c r="P49" s="11"/>
     </row>
     <row r="50" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L50" s="10" t="s">
+      <c r="L50" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M50" s="14">
+      <c r="M50" s="13">
         <v>238</v>
       </c>
-      <c r="N50" s="13">
+      <c r="N50" s="12">
         <v>678</v>
       </c>
-      <c r="O50" s="13" t="s">
+      <c r="O50" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="P50" s="13"/>
+      <c r="P50" s="12"/>
     </row>
     <row r="51" spans="12:16" x14ac:dyDescent="0.3">
       <c r="L51" s="1" t="s">

</xml_diff>

<commit_message>
Final draft, finish chapter 3, add abstract, keywords and bib
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JELENA\FAKS\3.godina\6.semestar\zavrsni\zavrsni-rad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872286AF-3008-492E-B7BE-FC1D6555916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF22FCFE-FE9E-4A70-ADD3-B26DF038DA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59AAA055-06BE-4089-858D-5DFDDCE26241}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t>d/cm</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>NE VALJA</t>
+  </si>
+  <si>
+    <t>bez filtra</t>
+  </si>
+  <si>
+    <t>s filtrom</t>
+  </si>
+  <si>
+    <t>trljbrlj</t>
   </si>
 </sst>
 </file>
@@ -211,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +269,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -288,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,6 +347,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1778,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AA949A-4943-4AB9-B017-E41F54B3B033}">
-  <dimension ref="F1:Q56"/>
+  <dimension ref="F1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1993,7 +2012,7 @@
         <v>-41</v>
       </c>
     </row>
-    <row r="17" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F17">
         <v>15</v>
       </c>
@@ -2004,7 +2023,7 @@
         <v>-31</v>
       </c>
     </row>
-    <row r="18" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F18">
         <v>16</v>
       </c>
@@ -2015,7 +2034,7 @@
         <v>-47</v>
       </c>
     </row>
-    <row r="19" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F19">
         <v>17</v>
       </c>
@@ -2026,7 +2045,7 @@
         <v>-42</v>
       </c>
     </row>
-    <row r="20" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F20">
         <v>18</v>
       </c>
@@ -2037,7 +2056,7 @@
         <v>-36</v>
       </c>
     </row>
-    <row r="21" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F21">
         <v>19</v>
       </c>
@@ -2048,7 +2067,7 @@
         <v>-34</v>
       </c>
     </row>
-    <row r="22" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F22">
         <v>20</v>
       </c>
@@ -2059,12 +2078,20 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="24" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="M23" t="s">
+        <v>46</v>
+      </c>
+      <c r="T23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="6:23" x14ac:dyDescent="0.3">
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:23" x14ac:dyDescent="0.3">
       <c r="L25" s="6" t="s">
         <v>6</v>
       </c>
@@ -2077,8 +2104,20 @@
       <c r="O25" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="S25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T25" s="7">
+        <v>1</v>
+      </c>
+      <c r="U25" s="7">
+        <v>2</v>
+      </c>
+      <c r="V25" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="6:23" x14ac:dyDescent="0.3">
       <c r="L26" s="1" t="s">
         <v>7</v>
       </c>
@@ -2091,8 +2130,14 @@
       <c r="O26">
         <v>645</v>
       </c>
-    </row>
-    <row r="27" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="S26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T26">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="27" spans="6:23" x14ac:dyDescent="0.3">
       <c r="L27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2105,8 +2150,20 @@
       <c r="O27">
         <v>1880</v>
       </c>
-    </row>
-    <row r="28" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="S27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T27">
+        <v>53</v>
+      </c>
+      <c r="U27" s="9">
+        <v>907</v>
+      </c>
+      <c r="V27">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="28" spans="6:23" x14ac:dyDescent="0.3">
       <c r="L28" s="1" t="s">
         <v>9</v>
       </c>
@@ -2119,8 +2176,26 @@
       <c r="O28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="S28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T28">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="29" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="G29" s="20">
+        <v>137</v>
+      </c>
+      <c r="H29" s="20">
+        <v>190</v>
+      </c>
+      <c r="I29" s="20">
+        <v>490</v>
+      </c>
+      <c r="J29" s="20">
+        <v>1243</v>
+      </c>
       <c r="L29" s="1" t="s">
         <v>10</v>
       </c>
@@ -2136,8 +2211,17 @@
       <c r="P29" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="S29" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="I30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="L30" s="1" t="s">
         <v>11</v>
       </c>
@@ -2150,8 +2234,20 @@
       <c r="O30" s="9">
         <v>1094</v>
       </c>
-    </row>
-    <row r="31" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="S30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T30">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="31" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="I31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="L31" s="1" t="s">
         <v>13</v>
       </c>
@@ -2164,8 +2260,20 @@
       <c r="O31" s="9">
         <v>991</v>
       </c>
-    </row>
-    <row r="32" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="S31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T31">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="32" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="I32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="L32" s="1" t="s">
         <v>12</v>
       </c>
@@ -2178,8 +2286,29 @@
       <c r="O32" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T32">
+        <v>431</v>
+      </c>
+      <c r="U32">
+        <v>903</v>
+      </c>
+      <c r="V32">
+        <v>1400</v>
+      </c>
+      <c r="W32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="I33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="L33" s="1" t="s">
         <v>14</v>
       </c>
@@ -2192,8 +2321,17 @@
       <c r="O33" s="9">
         <v>1479</v>
       </c>
-    </row>
-    <row r="34" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T33">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="34" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="J34" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="L34" s="1" t="s">
         <v>15</v>
       </c>
@@ -2209,8 +2347,23 @@
       <c r="P34" s="9">
         <v>1961</v>
       </c>
-    </row>
-    <row r="35" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T34">
+        <v>660</v>
+      </c>
+      <c r="U34" s="19">
+        <v>1224</v>
+      </c>
+      <c r="V34" s="9">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="35" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="J35" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="L35" s="1" t="s">
         <v>16</v>
       </c>
@@ -2223,8 +2376,23 @@
       <c r="O35" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T35">
+        <v>500</v>
+      </c>
+      <c r="U35" s="9">
+        <v>855</v>
+      </c>
+      <c r="V35">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="36" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="J36" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="L36" s="1" t="s">
         <v>17</v>
       </c>
@@ -2237,8 +2405,17 @@
       <c r="O36" s="9">
         <v>840</v>
       </c>
-    </row>
-    <row r="37" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T36">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="37" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="J37" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="L37" s="1" t="s">
         <v>18</v>
       </c>
@@ -2251,8 +2428,17 @@
       <c r="O37" s="9">
         <v>1448</v>
       </c>
-    </row>
-    <row r="38" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T37">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="38" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="J38" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="L38" s="1" t="s">
         <v>19</v>
       </c>
@@ -2265,8 +2451,17 @@
       <c r="O38">
         <v>1447</v>
       </c>
-    </row>
-    <row r="39" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T38">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="39" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="J39" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="L39" s="1" t="s">
         <v>20</v>
       </c>
@@ -2279,8 +2474,17 @@
       <c r="O39" s="9">
         <v>1316</v>
       </c>
-    </row>
-    <row r="40" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T39">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="40" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="J40" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="L40" s="1" t="s">
         <v>21</v>
       </c>
@@ -2296,8 +2500,17 @@
       <c r="P40" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T40">
+        <v>1313</v>
+      </c>
+      <c r="U40">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="41" spans="9:22" x14ac:dyDescent="0.3">
       <c r="L41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2310,8 +2523,14 @@
       <c r="O41">
         <v>947</v>
       </c>
-    </row>
-    <row r="42" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T41">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="42" spans="9:22" x14ac:dyDescent="0.3">
       <c r="L42" s="1" t="s">
         <v>23</v>
       </c>
@@ -2324,8 +2543,17 @@
       <c r="O42">
         <v>690</v>
       </c>
-    </row>
-    <row r="43" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T42">
+        <v>49</v>
+      </c>
+      <c r="U42">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="43" spans="9:22" x14ac:dyDescent="0.3">
       <c r="L43" s="1" t="s">
         <v>24</v>
       </c>
@@ -2338,8 +2566,14 @@
       <c r="O43">
         <v>1464</v>
       </c>
-    </row>
-    <row r="44" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T43">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="44" spans="9:22" x14ac:dyDescent="0.3">
       <c r="L44" s="1" t="s">
         <v>25</v>
       </c>
@@ -2352,8 +2586,14 @@
       <c r="O44">
         <v>903</v>
       </c>
-    </row>
-    <row r="45" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T44">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="45" spans="9:22" x14ac:dyDescent="0.3">
       <c r="L45" s="1" t="s">
         <v>26</v>
       </c>
@@ -2366,8 +2606,14 @@
       <c r="O45" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="46" spans="9:22" x14ac:dyDescent="0.3">
       <c r="L46" s="10" t="s">
         <v>27</v>
       </c>
@@ -2379,8 +2625,11 @@
       </c>
       <c r="O46" s="11"/>
       <c r="P46" s="11"/>
-    </row>
-    <row r="47" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S46" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="9:22" x14ac:dyDescent="0.3">
       <c r="L47" s="18" t="s">
         <v>28</v>
       </c>
@@ -2397,8 +2646,14 @@
       <c r="Q47" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="S47" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="T47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+    </row>
+    <row r="48" spans="9:22" x14ac:dyDescent="0.3">
       <c r="L48" s="1" t="s">
         <v>37</v>
       </c>
@@ -2411,8 +2666,14 @@
       <c r="O48" s="9">
         <v>1302</v>
       </c>
-    </row>
-    <row r="49" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="S48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T48">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="49" spans="12:21" x14ac:dyDescent="0.3">
       <c r="L49" s="10" t="s">
         <v>29</v>
       </c>
@@ -2424,8 +2685,11 @@
       </c>
       <c r="O49" s="11"/>
       <c r="P49" s="11"/>
-    </row>
-    <row r="50" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="S49" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="12:21" x14ac:dyDescent="0.3">
       <c r="L50" s="14" t="s">
         <v>30</v>
       </c>
@@ -2439,8 +2703,17 @@
         <v>38</v>
       </c>
       <c r="P50" s="12"/>
-    </row>
-    <row r="51" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="S50" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="T50">
+        <v>242</v>
+      </c>
+      <c r="U50">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="51" spans="12:21" x14ac:dyDescent="0.3">
       <c r="L51" s="1" t="s">
         <v>31</v>
       </c>
@@ -2453,8 +2726,17 @@
       <c r="O51" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="S51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T51">
+        <v>670</v>
+      </c>
+      <c r="U51">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="52" spans="12:21" x14ac:dyDescent="0.3">
       <c r="L52" s="1" t="s">
         <v>32</v>
       </c>
@@ -2464,8 +2746,14 @@
       <c r="N52" s="9">
         <v>1182</v>
       </c>
-    </row>
-    <row r="53" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="S52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T52">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="53" spans="12:21" x14ac:dyDescent="0.3">
       <c r="L53" s="1" t="s">
         <v>33</v>
       </c>
@@ -2481,8 +2769,14 @@
       <c r="P53" s="9">
         <v>907</v>
       </c>
-    </row>
-    <row r="54" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="S53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T53">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="54" spans="12:21" x14ac:dyDescent="0.3">
       <c r="L54" s="1" t="s">
         <v>34</v>
       </c>
@@ -2495,8 +2789,14 @@
       <c r="O54" s="9">
         <v>1873</v>
       </c>
-    </row>
-    <row r="55" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="S54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T54">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="55" spans="12:21" x14ac:dyDescent="0.3">
       <c r="L55" s="1" t="s">
         <v>35</v>
       </c>
@@ -2509,8 +2809,17 @@
       <c r="O55">
         <v>1468</v>
       </c>
-    </row>
-    <row r="56" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="S55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T55">
+        <v>49</v>
+      </c>
+      <c r="U55">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="56" spans="12:21" x14ac:dyDescent="0.3">
       <c r="L56" s="1" t="s">
         <v>36</v>
       </c>
@@ -2521,6 +2830,12 @@
         <v>500</v>
       </c>
       <c r="O56">
+        <v>908</v>
+      </c>
+      <c r="S56" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T56">
         <v>908</v>
       </c>
     </row>

</xml_diff>